<commit_message>
Adding truthy/falsy values in xlsx extractor
</commit_message>
<xml_diff>
--- a/src/test/resources/xlsx/example.xlsx
+++ b/src/test/resources/xlsx/example.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>metric1</t>
   </si>
@@ -28,6 +28,12 @@
   </si>
   <si>
     <t>metric3</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -399,7 +405,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -416,15 +422,15 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>2</v>
+      <c r="B2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="B3" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>